<commit_message>
sti uploada kaynaklar eklendi
</commit_message>
<xml_diff>
--- a/Wms12m.Presentation/Content/STISablon.xlsx
+++ b/Wms12m.Presentation/Content/STISablon.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>MalKodu</t>
   </si>
@@ -33,6 +33,18 @@
   </si>
   <si>
     <t>Birim</t>
+  </si>
+  <si>
+    <t>Kaynak Sipariş No</t>
+  </si>
+  <si>
+    <t>Kaynak Sipariş Sıra No</t>
+  </si>
+  <si>
+    <t>Kaynak Sipariş Tarih</t>
+  </si>
+  <si>
+    <t>Kaynak Sipariş Miktar</t>
   </si>
 </sst>
 </file>
@@ -377,21 +389,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" hidden="1"/>
+    <col min="2" max="2" width="9" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -401,9 +415,21 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="sZA3Sn8yyBF/TvhJIiDhOPmnaQ8Z32hPYdnC803xpiljlql7SGQ+TJWTng8X0MdJ69aOZYzduqc5Nf+vstWcig==" saltValue="uJK2kr7tOuwluac27JmZ/g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="X5n8ldBZYiPC0Dz82/kHDXiuCn6frEB6sr4uvpbAMRfdVAI8n2DgSxVlLTbBKxUP5wIhodoX7G5QbYtbMY53/w==" saltValue="vrkuSRMTnwT8hYqz4B1R7A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
sti yükleme modeli değişti
</commit_message>
<xml_diff>
--- a/Wms12m.Presentation/Content/STISablon.xlsx
+++ b/Wms12m.Presentation/Content/STISablon.xlsx
@@ -8,6 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Projects\ASP .NET\WMS\Wms12m.Presentation\Content\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="/ZQn01o6aOjaYa0C8nw+UuYcucs73LZrQX3R/ZIEyy8Ti9sL0ay6E27hSJxYtblwuuaO3d96aG7q0uQvdaUgYQ==" workbookSaltValue="ZTcmqO6MCl2Oi8LPwW+m3Q==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9615"/>
   </bookViews>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>MalKodu</t>
   </si>
@@ -38,13 +39,7 @@
     <t>Kaynak Sipariş No</t>
   </si>
   <si>
-    <t>Kaynak Sipariş Sıra No</t>
-  </si>
-  <si>
-    <t>Kaynak Sipariş Tarih</t>
-  </si>
-  <si>
-    <t>Kaynak Sipariş Miktar</t>
+    <t>İrsaliye No</t>
   </si>
 </sst>
 </file>
@@ -99,7 +94,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -107,6 +102,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -389,47 +387,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="9" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="1" width="18.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="1" customWidth="1"/>
+    <col min="6" max="8" width="0" hidden="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="X5n8ldBZYiPC0Dz82/kHDXiuCn6frEB6sr4uvpbAMRfdVAI8n2DgSxVlLTbBKxUP5wIhodoX7G5QbYtbMY53/w==" saltValue="vrkuSRMTnwT8hYqz4B1R7A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Rby5CmCH8PkYvuDy6Kj7RM+yUM3FLeRVJUU4Kvkq3XZOGJF5pWeX+RuAsSRgZC7DOHGFjdUXgiY6/AgX5RnArg==" saltValue="ZTosSsfoin+3L3P+gqlPTw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>